<commit_message>
Notes and examples variables
</commit_message>
<xml_diff>
--- a/Updates.xlsx
+++ b/Updates.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26327"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Java Full Stack\JAVA\CORE\KTG\Ranjith\2023 march batch\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{259BF8FD-013D-4ED9-9573-4ED8738898A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54BACEDC-1531-4A26-AC78-5AE9D0E257FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="48">
   <si>
     <t>Concepts</t>
   </si>
@@ -98,6 +98,78 @@
   </si>
   <si>
     <t>JavaScript basics and arrays done</t>
+  </si>
+  <si>
+    <t>day-6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">js advanced </t>
+  </si>
+  <si>
+    <t>js validations,</t>
+  </si>
+  <si>
+    <t>Bootstrap</t>
+  </si>
+  <si>
+    <t>9:30PM-10:20PM</t>
+  </si>
+  <si>
+    <t>Typescript</t>
+  </si>
+  <si>
+    <t>9:00pm-10:00pm</t>
+  </si>
+  <si>
+    <t>Angular intro</t>
+  </si>
+  <si>
+    <t>Angular components,commands ,basic structure</t>
+  </si>
+  <si>
+    <t>9:05-10:00pm</t>
+  </si>
+  <si>
+    <t>routing ,directives,data binding ….</t>
+  </si>
+  <si>
+    <t>9:00-10:05pm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">direcgtives revise </t>
+  </si>
+  <si>
+    <t xml:space="preserve">pipes,forms </t>
+  </si>
+  <si>
+    <t>authguards</t>
+  </si>
+  <si>
+    <t>Json files,services,crud operations json…,httpclient</t>
+  </si>
+  <si>
+    <t>9:45PM-10:25Pm</t>
+  </si>
+  <si>
+    <t>10:30PM -11:30PM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">complete java setup  and eclipse </t>
+  </si>
+  <si>
+    <t>Java Intro,java setup</t>
+  </si>
+  <si>
+    <t>execution flow,basic variables,identifiers</t>
+  </si>
+  <si>
+    <t>10:30PM -11:25PM</t>
+  </si>
+  <si>
+    <t>Variables,datatypes,Eclipse</t>
+  </si>
+  <si>
+    <t>Variables instance,static</t>
   </si>
 </sst>
 </file>
@@ -539,8 +611,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A3:I166"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="H23" sqref="H23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -549,7 +621,7 @@
     <col min="5" max="5" width="19" customWidth="1"/>
     <col min="6" max="6" width="43" customWidth="1"/>
     <col min="7" max="7" width="30.109375" customWidth="1"/>
-    <col min="8" max="8" width="23.6640625" customWidth="1"/>
+    <col min="8" max="8" width="32.33203125" customWidth="1"/>
     <col min="9" max="9" width="60.77734375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -665,115 +737,201 @@
       <c r="I9" s="5"/>
     </row>
     <row r="10" spans="4:9" x14ac:dyDescent="0.3">
-      <c r="D10" s="4"/>
-      <c r="E10" s="6"/>
-      <c r="F10" s="5"/>
-      <c r="G10" s="5"/>
+      <c r="D10" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="E10" s="6">
+        <v>45015</v>
+      </c>
+      <c r="F10" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="G10" s="11" t="s">
+        <v>19</v>
+      </c>
       <c r="H10" s="5"/>
       <c r="I10" s="5"/>
     </row>
     <row r="11" spans="4:9" x14ac:dyDescent="0.3">
       <c r="D11" s="4"/>
-      <c r="E11" s="6"/>
-      <c r="F11" s="5"/>
-      <c r="G11" s="5"/>
+      <c r="E11" s="6">
+        <v>45016</v>
+      </c>
+      <c r="F11" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="G11" s="11" t="s">
+        <v>19</v>
+      </c>
       <c r="H11" s="5"/>
       <c r="I11" s="5"/>
     </row>
     <row r="12" spans="4:9" x14ac:dyDescent="0.3">
       <c r="D12" s="4"/>
-      <c r="E12" s="6"/>
-      <c r="F12" s="5"/>
-      <c r="G12" s="5"/>
+      <c r="E12" s="6">
+        <v>45019</v>
+      </c>
+      <c r="F12" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="G12" s="5" t="s">
+        <v>28</v>
+      </c>
       <c r="H12" s="5"/>
       <c r="I12" s="5"/>
     </row>
     <row r="13" spans="4:9" x14ac:dyDescent="0.3">
       <c r="D13" s="4"/>
-      <c r="E13" s="6"/>
-      <c r="F13" s="5"/>
-      <c r="G13" s="5"/>
+      <c r="E13" s="6">
+        <v>45022</v>
+      </c>
+      <c r="F13" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="G13" s="5" t="s">
+        <v>30</v>
+      </c>
       <c r="H13" s="5"/>
       <c r="I13" s="5"/>
     </row>
     <row r="14" spans="4:9" x14ac:dyDescent="0.3">
       <c r="D14" s="4"/>
-      <c r="E14" s="8"/>
-      <c r="F14" s="5"/>
-      <c r="G14" s="7"/>
+      <c r="E14" s="6">
+        <v>45023</v>
+      </c>
+      <c r="F14" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="G14" s="5" t="s">
+        <v>30</v>
+      </c>
       <c r="H14" s="5"/>
       <c r="I14" s="5"/>
     </row>
     <row r="15" spans="4:9" x14ac:dyDescent="0.3">
       <c r="D15" s="4"/>
-      <c r="E15" s="8"/>
-      <c r="F15" s="5"/>
-      <c r="G15" s="5"/>
+      <c r="E15" s="8">
+        <v>45026</v>
+      </c>
+      <c r="F15" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="G15" s="5" t="s">
+        <v>33</v>
+      </c>
       <c r="H15" s="5"/>
       <c r="I15" s="5"/>
     </row>
     <row r="16" spans="4:9" x14ac:dyDescent="0.3">
       <c r="D16" s="4"/>
-      <c r="E16" s="8"/>
-      <c r="F16" s="5"/>
-      <c r="G16" s="5"/>
-      <c r="H16" s="5"/>
+      <c r="E16" s="8">
+        <v>45027</v>
+      </c>
+      <c r="F16" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="G16" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="H16" s="5" t="s">
+        <v>36</v>
+      </c>
       <c r="I16" s="5"/>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="D17" s="4"/>
-      <c r="E17" s="8"/>
-      <c r="F17" s="5"/>
+      <c r="E17" s="8">
+        <v>45028</v>
+      </c>
+      <c r="F17" s="5" t="s">
+        <v>37</v>
+      </c>
       <c r="G17" s="5"/>
       <c r="H17" s="5"/>
       <c r="I17" s="5"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="D18" s="4"/>
-      <c r="E18" s="8"/>
-      <c r="F18" s="5"/>
+      <c r="E18" s="8">
+        <v>45035</v>
+      </c>
+      <c r="F18" s="5" t="s">
+        <v>38</v>
+      </c>
       <c r="G18" s="7"/>
       <c r="H18" s="5"/>
       <c r="I18" s="5"/>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="D19" s="4"/>
-      <c r="E19" s="8"/>
-      <c r="F19" s="5"/>
-      <c r="G19" s="7"/>
+      <c r="E19" s="8">
+        <v>45040</v>
+      </c>
+      <c r="F19" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="G19" s="7" t="s">
+        <v>40</v>
+      </c>
       <c r="H19" s="5"/>
       <c r="I19" s="5"/>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A20" s="9"/>
       <c r="D20" s="4"/>
-      <c r="E20" s="8"/>
-      <c r="F20" s="5"/>
-      <c r="G20" s="5"/>
-      <c r="H20" s="5"/>
+      <c r="E20" s="8">
+        <v>45042</v>
+      </c>
+      <c r="F20" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="G20" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="H20" s="5" t="s">
+        <v>42</v>
+      </c>
       <c r="I20" s="5"/>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.3">
       <c r="D21" s="4"/>
-      <c r="E21" s="8"/>
-      <c r="F21" s="5"/>
-      <c r="G21" s="7"/>
+      <c r="E21" s="8">
+        <v>45044</v>
+      </c>
+      <c r="F21" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="G21" s="5" t="s">
+        <v>45</v>
+      </c>
       <c r="H21" s="5"/>
       <c r="I21" s="5"/>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.3">
       <c r="D22" s="4"/>
-      <c r="E22" s="5"/>
-      <c r="F22" s="5"/>
-      <c r="G22" s="5"/>
+      <c r="E22" s="8">
+        <v>45048</v>
+      </c>
+      <c r="F22" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="G22" s="5" t="s">
+        <v>45</v>
+      </c>
       <c r="H22" s="5"/>
       <c r="I22" s="5"/>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.3">
       <c r="D23" s="4"/>
-      <c r="E23" s="5"/>
-      <c r="F23" s="5"/>
-      <c r="G23" s="5"/>
+      <c r="E23" s="8">
+        <v>45051</v>
+      </c>
+      <c r="F23" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="G23" s="5" t="s">
+        <v>41</v>
+      </c>
       <c r="H23" s="5"/>
       <c r="I23" s="5"/>
     </row>

</xml_diff>